<commit_message>
categorys with icons appear to be working.  Thinly tested
</commit_message>
<xml_diff>
--- a/tools/categories/categorymap.xlsx
+++ b/tools/categories/categorymap.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="50460" windowHeight="28360" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30220" windowHeight="25940" tabRatio="549" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Map_Candi_Foursquare" sheetId="8" r:id="rId1"/>
-    <sheet name="Map_Factual_Foursquare" sheetId="1" r:id="rId2"/>
-    <sheet name="Map_Google_Foursquare" sheetId="6" r:id="rId3"/>
-    <sheet name="Foursquare" sheetId="3" r:id="rId4"/>
-    <sheet name="Factual" sheetId="4" r:id="rId5"/>
-    <sheet name="Google" sheetId="5" r:id="rId6"/>
-    <sheet name="Candi" sheetId="7" r:id="rId7"/>
+    <sheet name="map_candi_foursquare" sheetId="8" r:id="rId1"/>
+    <sheet name="map_factual_foursquare" sheetId="1" r:id="rId2"/>
+    <sheet name="map_google_foursquare" sheetId="6" r:id="rId3"/>
+    <sheet name="foursquare" sheetId="3" r:id="rId4"/>
+    <sheet name="factual" sheetId="4" r:id="rId5"/>
+    <sheet name="google" sheetId="5" r:id="rId6"/>
+    <sheet name="candi" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4921" uniqueCount="1592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5017" uniqueCount="1540">
   <si>
     <t>4fceea171983d5d06c3e9823</t>
   </si>
@@ -4645,169 +4645,13 @@
   </si>
   <si>
     <t>video_games</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931737</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931738</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931739</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931740</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931741</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931742</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931743</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931744</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931745</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931746</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931747</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931748</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931749</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931750</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931751</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931752</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931753</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931754</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931755</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931756</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931757</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931758</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931759</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931760</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931761</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931762</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931763</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931764</t>
-  </si>
-  <si>
-    <t>4bf58dd8d48988d1ff931765</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81260</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81261</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81262</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81263</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81264</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81265</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81266</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81267</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81268</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81269</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81270</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81271</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81272</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81273</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81274</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81275</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81276</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81277</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81278</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81279</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81280</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81281</t>
-  </si>
-  <si>
-    <t>4d4b7105d754a06375d81282</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4843,6 +4687,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4861,7 +4712,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4879,15 +4730,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4896,6 +4758,11 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4904,6 +4771,11 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5236,15 +5108,16 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5255,7 +5128,7 @@
         <v>1441</v>
       </c>
       <c r="C1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D1" t="s">
         <v>483</v>
@@ -5271,7 +5144,7 @@
       <c r="B2" t="s">
         <v>1442</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>574</v>
       </c>
       <c r="D2" t="s">
@@ -5289,7 +5162,7 @@
         <v>1443</v>
       </c>
       <c r="C3" t="s">
-        <v>1540</v>
+        <v>482</v>
       </c>
       <c r="D3" t="s">
         <v>483</v>
@@ -5306,7 +5179,7 @@
         <v>531</v>
       </c>
       <c r="C4" t="s">
-        <v>1541</v>
+        <v>482</v>
       </c>
       <c r="D4" t="s">
         <v>483</v>
@@ -5323,7 +5196,7 @@
         <v>1444</v>
       </c>
       <c r="C5" t="s">
-        <v>1542</v>
+        <v>482</v>
       </c>
       <c r="D5" t="s">
         <v>483</v>
@@ -5340,7 +5213,7 @@
         <v>1445</v>
       </c>
       <c r="C6" t="s">
-        <v>1543</v>
+        <v>482</v>
       </c>
       <c r="D6" t="s">
         <v>483</v>
@@ -5357,7 +5230,7 @@
         <v>535</v>
       </c>
       <c r="C7" t="s">
-        <v>1544</v>
+        <v>482</v>
       </c>
       <c r="D7" t="s">
         <v>483</v>
@@ -5374,7 +5247,7 @@
         <v>1446</v>
       </c>
       <c r="C8" t="s">
-        <v>1545</v>
+        <v>482</v>
       </c>
       <c r="D8" t="s">
         <v>483</v>
@@ -5391,7 +5264,7 @@
         <v>1447</v>
       </c>
       <c r="C9" t="s">
-        <v>1546</v>
+        <v>482</v>
       </c>
       <c r="D9" t="s">
         <v>483</v>
@@ -5408,7 +5281,7 @@
         <v>1448</v>
       </c>
       <c r="C10" t="s">
-        <v>1547</v>
+        <v>482</v>
       </c>
       <c r="D10" t="s">
         <v>483</v>
@@ -5425,7 +5298,7 @@
         <v>1449</v>
       </c>
       <c r="C11" t="s">
-        <v>1548</v>
+        <v>482</v>
       </c>
       <c r="D11" t="s">
         <v>483</v>
@@ -5442,7 +5315,7 @@
         <v>1450</v>
       </c>
       <c r="C12" t="s">
-        <v>1549</v>
+        <v>482</v>
       </c>
       <c r="D12" t="s">
         <v>483</v>
@@ -5459,7 +5332,7 @@
         <v>1451</v>
       </c>
       <c r="C13" t="s">
-        <v>1550</v>
+        <v>482</v>
       </c>
       <c r="D13" t="s">
         <v>483</v>
@@ -5476,7 +5349,7 @@
         <v>1452</v>
       </c>
       <c r="C14" t="s">
-        <v>1551</v>
+        <v>482</v>
       </c>
       <c r="D14" t="s">
         <v>483</v>
@@ -5493,7 +5366,7 @@
         <v>1453</v>
       </c>
       <c r="C15" t="s">
-        <v>1552</v>
+        <v>482</v>
       </c>
       <c r="D15" t="s">
         <v>483</v>
@@ -5510,7 +5383,7 @@
         <v>1454</v>
       </c>
       <c r="C16" t="s">
-        <v>1553</v>
+        <v>482</v>
       </c>
       <c r="D16" t="s">
         <v>483</v>
@@ -5527,7 +5400,7 @@
         <v>519</v>
       </c>
       <c r="C17" t="s">
-        <v>1554</v>
+        <v>482</v>
       </c>
       <c r="D17" t="s">
         <v>483</v>
@@ -5544,7 +5417,7 @@
         <v>1455</v>
       </c>
       <c r="C18" t="s">
-        <v>1555</v>
+        <v>482</v>
       </c>
       <c r="D18" t="s">
         <v>483</v>
@@ -5561,7 +5434,7 @@
         <v>355</v>
       </c>
       <c r="C19" t="s">
-        <v>1556</v>
+        <v>482</v>
       </c>
       <c r="D19" t="s">
         <v>483</v>
@@ -5578,7 +5451,7 @@
         <v>1456</v>
       </c>
       <c r="C20" t="s">
-        <v>1557</v>
+        <v>482</v>
       </c>
       <c r="D20" t="s">
         <v>483</v>
@@ -5595,7 +5468,7 @@
         <v>1457</v>
       </c>
       <c r="C21" t="s">
-        <v>1558</v>
+        <v>482</v>
       </c>
       <c r="D21" t="s">
         <v>483</v>
@@ -5612,7 +5485,7 @@
         <v>483</v>
       </c>
       <c r="C22" t="s">
-        <v>1559</v>
+        <v>482</v>
       </c>
       <c r="D22" t="s">
         <v>483</v>
@@ -5629,7 +5502,7 @@
         <v>1458</v>
       </c>
       <c r="C23" t="s">
-        <v>1560</v>
+        <v>482</v>
       </c>
       <c r="D23" t="s">
         <v>483</v>
@@ -5646,7 +5519,7 @@
         <v>541</v>
       </c>
       <c r="C24" t="s">
-        <v>1561</v>
+        <v>482</v>
       </c>
       <c r="D24" t="s">
         <v>483</v>
@@ -5663,7 +5536,7 @@
         <v>1459</v>
       </c>
       <c r="C25" t="s">
-        <v>1562</v>
+        <v>482</v>
       </c>
       <c r="D25" t="s">
         <v>483</v>
@@ -5680,7 +5553,7 @@
         <v>1460</v>
       </c>
       <c r="C26" t="s">
-        <v>1563</v>
+        <v>482</v>
       </c>
       <c r="D26" t="s">
         <v>483</v>
@@ -5697,7 +5570,7 @@
         <v>1461</v>
       </c>
       <c r="C27" t="s">
-        <v>1564</v>
+        <v>482</v>
       </c>
       <c r="D27" t="s">
         <v>483</v>
@@ -5714,7 +5587,7 @@
         <v>1462</v>
       </c>
       <c r="C28" t="s">
-        <v>1565</v>
+        <v>482</v>
       </c>
       <c r="D28" t="s">
         <v>483</v>
@@ -5731,7 +5604,7 @@
         <v>1463</v>
       </c>
       <c r="C29" t="s">
-        <v>1566</v>
+        <v>482</v>
       </c>
       <c r="D29" t="s">
         <v>483</v>
@@ -5748,7 +5621,7 @@
         <v>1464</v>
       </c>
       <c r="C30" t="s">
-        <v>1567</v>
+        <v>482</v>
       </c>
       <c r="D30" t="s">
         <v>483</v>
@@ -5765,7 +5638,7 @@
         <v>1465</v>
       </c>
       <c r="C31" t="s">
-        <v>1568</v>
+        <v>482</v>
       </c>
       <c r="D31" t="s">
         <v>483</v>
@@ -5799,7 +5672,7 @@
         <v>1467</v>
       </c>
       <c r="C33" t="s">
-        <v>1569</v>
+        <v>574</v>
       </c>
       <c r="D33" t="s">
         <v>575</v>
@@ -5816,7 +5689,7 @@
         <v>1468</v>
       </c>
       <c r="C34" t="s">
-        <v>1570</v>
+        <v>574</v>
       </c>
       <c r="D34" t="s">
         <v>575</v>
@@ -5833,7 +5706,7 @@
         <v>1469</v>
       </c>
       <c r="C35" t="s">
-        <v>1571</v>
+        <v>574</v>
       </c>
       <c r="D35" t="s">
         <v>575</v>
@@ -5850,7 +5723,7 @@
         <v>969</v>
       </c>
       <c r="C36" t="s">
-        <v>1572</v>
+        <v>574</v>
       </c>
       <c r="D36" t="s">
         <v>575</v>
@@ -5867,7 +5740,7 @@
         <v>1470</v>
       </c>
       <c r="C37" t="s">
-        <v>1573</v>
+        <v>574</v>
       </c>
       <c r="D37" t="s">
         <v>575</v>
@@ -5884,7 +5757,7 @@
         <v>862</v>
       </c>
       <c r="C38" t="s">
-        <v>1574</v>
+        <v>574</v>
       </c>
       <c r="D38" t="s">
         <v>575</v>
@@ -5901,7 +5774,7 @@
         <v>1471</v>
       </c>
       <c r="C39" t="s">
-        <v>1575</v>
+        <v>574</v>
       </c>
       <c r="D39" t="s">
         <v>575</v>
@@ -5918,7 +5791,7 @@
         <v>1472</v>
       </c>
       <c r="C40" t="s">
-        <v>1576</v>
+        <v>574</v>
       </c>
       <c r="D40" t="s">
         <v>575</v>
@@ -5935,7 +5808,7 @@
         <v>1473</v>
       </c>
       <c r="C41" t="s">
-        <v>1577</v>
+        <v>574</v>
       </c>
       <c r="D41" t="s">
         <v>575</v>
@@ -5952,7 +5825,7 @@
         <v>1474</v>
       </c>
       <c r="C42" t="s">
-        <v>1578</v>
+        <v>574</v>
       </c>
       <c r="D42" t="s">
         <v>575</v>
@@ -5969,7 +5842,7 @@
         <v>1475</v>
       </c>
       <c r="C43" t="s">
-        <v>1579</v>
+        <v>574</v>
       </c>
       <c r="D43" t="s">
         <v>575</v>
@@ -5986,7 +5859,7 @@
         <v>1476</v>
       </c>
       <c r="C44" t="s">
-        <v>1580</v>
+        <v>574</v>
       </c>
       <c r="D44" t="s">
         <v>575</v>
@@ -6003,7 +5876,7 @@
         <v>1477</v>
       </c>
       <c r="C45" t="s">
-        <v>1581</v>
+        <v>574</v>
       </c>
       <c r="D45" t="s">
         <v>575</v>
@@ -6020,7 +5893,7 @@
         <v>1478</v>
       </c>
       <c r="C46" t="s">
-        <v>1582</v>
+        <v>574</v>
       </c>
       <c r="D46" t="s">
         <v>575</v>
@@ -6037,7 +5910,7 @@
         <v>998</v>
       </c>
       <c r="C47" t="s">
-        <v>1583</v>
+        <v>574</v>
       </c>
       <c r="D47" t="s">
         <v>575</v>
@@ -6054,7 +5927,7 @@
         <v>1479</v>
       </c>
       <c r="C48" t="s">
-        <v>1584</v>
+        <v>574</v>
       </c>
       <c r="D48" t="s">
         <v>575</v>
@@ -6071,7 +5944,7 @@
         <v>1480</v>
       </c>
       <c r="C49" t="s">
-        <v>1585</v>
+        <v>574</v>
       </c>
       <c r="D49" t="s">
         <v>575</v>
@@ -6088,7 +5961,7 @@
         <v>1481</v>
       </c>
       <c r="C50" t="s">
-        <v>1586</v>
+        <v>574</v>
       </c>
       <c r="D50" t="s">
         <v>575</v>
@@ -6105,7 +5978,7 @@
         <v>1482</v>
       </c>
       <c r="C51" t="s">
-        <v>1587</v>
+        <v>574</v>
       </c>
       <c r="D51" t="s">
         <v>575</v>
@@ -6122,7 +5995,7 @@
         <v>1205</v>
       </c>
       <c r="C52" t="s">
-        <v>1588</v>
+        <v>574</v>
       </c>
       <c r="D52" t="s">
         <v>575</v>
@@ -6139,7 +6012,7 @@
         <v>1483</v>
       </c>
       <c r="C53" t="s">
-        <v>1589</v>
+        <v>574</v>
       </c>
       <c r="D53" t="s">
         <v>575</v>
@@ -6156,7 +6029,7 @@
         <v>972</v>
       </c>
       <c r="C54" t="s">
-        <v>1590</v>
+        <v>574</v>
       </c>
       <c r="D54" t="s">
         <v>575</v>
@@ -6173,7 +6046,7 @@
         <v>1484</v>
       </c>
       <c r="C55" t="s">
-        <v>1591</v>
+        <v>574</v>
       </c>
       <c r="D55" t="s">
         <v>575</v>
@@ -13687,1360 +13560,1651 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>1277</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>1278</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>779</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>1279</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>1280</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>1281</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>1282</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>1284</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>1285</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>1286</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>1287</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>1288</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
         <v>1289</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>1290</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>785</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
         <v>1291</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>1292</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>1293</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>1294</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>816</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>817</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>1295</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
         <v>1296</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>1297</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>1298</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
         <v>1299</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
         <v>1300</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>1301</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>1302</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
         <v>1303</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>1304</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
         <v>1305</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
         <v>1306</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
         <v>1307</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>1308</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
         <v>1309</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>787</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
         <v>1310</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
         <v>1311</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
         <v>1312</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" s="4" t="s">
         <v>1313</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" s="4" t="s">
         <v>1314</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" s="4" t="s">
         <v>1315</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" s="4" t="s">
         <v>1316</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" s="4" t="s">
         <v>1317</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" s="4" t="s">
         <v>1318</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" s="4" t="s">
         <v>1319</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" s="4" t="s">
         <v>1320</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" s="4" t="s">
         <v>1321</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" s="4" t="s">
         <v>1322</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" s="4" t="s">
         <v>1323</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>664</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" s="4" t="s">
         <v>1324</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49" s="4" t="s">
         <v>1325</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
         <v>1326</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51" s="4" t="s">
         <v>1327</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
         <v>1328</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>704</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>705</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
         <v>1329</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>707</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="E53" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
         <v>1330</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55" s="4" t="s">
         <v>1331</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="A56" s="4" t="s">
         <v>1332</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="E56" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
         <v>1333</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
         <v>1334</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="E58" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="A59" s="4" t="s">
         <v>1335</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>810</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>811</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:5">
       <c r="A60" s="4" t="s">
         <v>1336</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="E60" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="A61" s="4" t="s">
         <v>1337</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="E61" s="4" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="A62" s="4" t="s">
         <v>1338</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="E62" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
         <v>1339</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>762</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="E63" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64" s="4" t="s">
         <v>1340</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65" s="4" t="s">
         <v>1341</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="E65" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66" s="4" t="s">
         <v>1342</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="E66" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67" s="4" t="s">
         <v>1343</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="E67" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:5">
       <c r="A68" s="4" t="s">
         <v>1344</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="E68" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="A69" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="E69" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70" s="4" t="s">
         <v>1346</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="E70" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71" s="4" t="s">
         <v>1347</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>728</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="A72" s="4" t="s">
         <v>1348</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="E72" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:5">
       <c r="A73" s="4" t="s">
         <v>1349</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="E73" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:5">
       <c r="A74" s="4" t="s">
         <v>1350</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="E74" s="4" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75" s="4" t="s">
         <v>1351</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="A76" s="4" t="s">
         <v>1352</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="D76" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="E76" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="A77" s="4" t="s">
         <v>1353</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="E77" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:5">
       <c r="A78" s="4" t="s">
         <v>1354</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>733</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="E78" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:5">
       <c r="A79" s="4" t="s">
         <v>1355</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="E79" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:5">
       <c r="A80" s="4" t="s">
         <v>1356</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>808</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="D80" s="3" t="s">
         <v>809</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="E80" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:5">
       <c r="A81" s="4" t="s">
         <v>1357</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="D81" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="E81" s="4" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:5">
       <c r="A82" s="4" t="s">
         <v>1358</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="E82" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:5">
       <c r="A83" s="4" t="s">
         <v>1359</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="E83" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:5">
       <c r="A84" s="4" t="s">
         <v>1360</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="E84" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:5">
       <c r="A85" s="4" t="s">
         <v>1361</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="D85" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="E85" s="4" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:5">
       <c r="A86" s="4" t="s">
         <v>1362</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="D86" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="E86" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:5">
       <c r="A87" s="4" t="s">
         <v>1363</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="D87" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="E87" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:5">
       <c r="A88" s="4" t="s">
         <v>1364</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="D88" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="E88" s="4" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:5">
       <c r="A89" s="4" t="s">
         <v>1365</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>822</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="D89" s="3" t="s">
         <v>823</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="E89" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:5">
       <c r="A90" s="4" t="s">
         <v>1366</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="D90" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="E90" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:5">
       <c r="A91" s="4" t="s">
         <v>1367</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="2" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="D91" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="E91" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:5">
       <c r="A92" s="4" t="s">
         <v>1368</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>832</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="D92" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:5">
       <c r="A93" s="4" t="s">
         <v>1369</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="D93" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="E93" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:5">
       <c r="A94" s="4" t="s">
         <v>1370</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="D94" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="E94" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:5">
       <c r="A95" s="4" t="s">
         <v>1371</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="E95" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:5">
       <c r="A96" s="4" t="s">
         <v>1372</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="E96" s="4" t="s">
         <v>1272</v>
       </c>
     </row>
@@ -15059,8 +15223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D419"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="G309" sqref="G309"/>
+    <sheetView showRuler="0" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25764,7 +25928,7 @@
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26557,7 +26721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- wip on patch categories.
</commit_message>
<xml_diff>
--- a/tools/categories/categorymap.xlsx
+++ b/tools/categories/categorymap.xlsx
@@ -5,23 +5,25 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Aircandi\Proxibase\tools\categories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Proxibase\tools\categories\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="285" windowWidth="27495" windowHeight="17880" tabRatio="654" activeTab="7"/>
+    <workbookView xWindow="4395" yWindow="285" windowWidth="27495" windowHeight="17880" tabRatio="654" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="map_candi_candi" sheetId="8" r:id="rId1"/>
     <sheet name="map_factual_candi" sheetId="1" r:id="rId2"/>
     <sheet name="map_google_candi" sheetId="6" r:id="rId3"/>
     <sheet name="map_foursquare_candi" sheetId="9" r:id="rId4"/>
-    <sheet name="foursquare" sheetId="3" r:id="rId5"/>
-    <sheet name="factual" sheetId="4" r:id="rId6"/>
-    <sheet name="google" sheetId="5" r:id="rId7"/>
-    <sheet name="candi" sheetId="7" r:id="rId8"/>
+    <sheet name="map_patches_candi" sheetId="10" r:id="rId5"/>
+    <sheet name="foursquare" sheetId="3" r:id="rId6"/>
+    <sheet name="factual" sheetId="4" r:id="rId7"/>
+    <sheet name="google" sheetId="5" r:id="rId8"/>
+    <sheet name="candi" sheetId="7" r:id="rId9"/>
+    <sheet name="patches" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130407"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6677" uniqueCount="1579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7182" uniqueCount="1603">
   <si>
     <t>Shopping</t>
   </si>
@@ -4790,13 +4792,97 @@
   </si>
   <si>
     <t>Home</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Pool Party</t>
+  </si>
+  <si>
+    <t>Birthday Party</t>
+  </si>
+  <si>
+    <t>Holiday Party</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Concert</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Birthday Parties (adult or children)</t>
+  </si>
+  <si>
+    <t>Theme Parties</t>
+  </si>
+  <si>
+    <t>Holiday Parties</t>
+  </si>
+  <si>
+    <t>Anniversaries</t>
+  </si>
+  <si>
+    <t>Retirements</t>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>weet Sixteen</t>
+    </r>
+  </si>
+  <si>
+    <t>Family Reunions</t>
+  </si>
+  <si>
+    <t>Fundraisers</t>
+  </si>
+  <si>
+    <t>Bachelor/Bachelorette Parties</t>
+  </si>
+  <si>
+    <t>Bridal Showers</t>
+  </si>
+  <si>
+    <t>Baby Showers</t>
+  </si>
+  <si>
+    <t>Cocktail Parties</t>
+  </si>
+  <si>
+    <t>Casino Party</t>
+  </si>
+  <si>
+    <t>Sleep Overs</t>
+  </si>
+  <si>
+    <t>Pool Parties</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4847,6 +4933,13 @@
       <sz val="13"/>
       <color indexed="63"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5223,7 +5316,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B25" sqref="A1:XFD1048576"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6180,12 +6273,825 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L51"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1583</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1579</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>210</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1583</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1579</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>210</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1583</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1579</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>210</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1583</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1584</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>210</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1585</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>210</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1586</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>210</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1587</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>210</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>210</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>210</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>210</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>210</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>210</v>
+      </c>
+      <c r="L20" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>210</v>
+      </c>
+      <c r="L21" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>210</v>
+      </c>
+      <c r="L22" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>210</v>
+      </c>
+      <c r="L23" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>210</v>
+      </c>
+      <c r="L24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>210</v>
+      </c>
+      <c r="L25" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>210</v>
+      </c>
+      <c r="L26" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="16.5">
+      <c r="A32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16.5">
+      <c r="A33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16.5">
+      <c r="A34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16.5">
+      <c r="A35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16.5">
+      <c r="A36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16.5">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.5">
+      <c r="A38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16.5">
+      <c r="A39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16.5">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16.5">
+      <c r="A41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16.5">
+      <c r="A42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16.5">
+      <c r="A43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16.5">
+      <c r="A44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16.5">
+      <c r="A45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16.5">
+      <c r="A46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16.5">
+      <c r="A47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16.5">
+      <c r="A48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="16.5">
+      <c r="A49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16.5">
+      <c r="A50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16.5">
+      <c r="A51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E439"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -13677,7 +14583,7 @@
   <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5"/>
@@ -21226,10 +22132,967 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>981</v>
+      </c>
+      <c r="D2" t="s">
+        <v>982</v>
+      </c>
+      <c r="E2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E17" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E20" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E25" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E30" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>981</v>
+      </c>
+      <c r="D32" t="s">
+        <v>982</v>
+      </c>
+      <c r="E32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>981</v>
+      </c>
+      <c r="D33" t="s">
+        <v>982</v>
+      </c>
+      <c r="E33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>981</v>
+      </c>
+      <c r="D34" t="s">
+        <v>982</v>
+      </c>
+      <c r="E34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>981</v>
+      </c>
+      <c r="D35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E35" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" t="s">
+        <v>547</v>
+      </c>
+      <c r="C36" t="s">
+        <v>981</v>
+      </c>
+      <c r="D36" t="s">
+        <v>982</v>
+      </c>
+      <c r="E36" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>981</v>
+      </c>
+      <c r="D37" t="s">
+        <v>982</v>
+      </c>
+      <c r="E37" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>791</v>
+      </c>
+      <c r="C38" t="s">
+        <v>981</v>
+      </c>
+      <c r="D38" t="s">
+        <v>982</v>
+      </c>
+      <c r="E38" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="s">
+        <v>981</v>
+      </c>
+      <c r="D39" t="s">
+        <v>982</v>
+      </c>
+      <c r="E39" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>981</v>
+      </c>
+      <c r="D40" t="s">
+        <v>982</v>
+      </c>
+      <c r="E40" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" t="s">
+        <v>981</v>
+      </c>
+      <c r="D41" t="s">
+        <v>982</v>
+      </c>
+      <c r="E41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>981</v>
+      </c>
+      <c r="D42" t="s">
+        <v>982</v>
+      </c>
+      <c r="E42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" t="s">
+        <v>981</v>
+      </c>
+      <c r="D43" t="s">
+        <v>982</v>
+      </c>
+      <c r="E43" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>981</v>
+      </c>
+      <c r="D44" t="s">
+        <v>982</v>
+      </c>
+      <c r="E44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>981</v>
+      </c>
+      <c r="D45" t="s">
+        <v>982</v>
+      </c>
+      <c r="E45" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s">
+        <v>981</v>
+      </c>
+      <c r="D46" t="s">
+        <v>982</v>
+      </c>
+      <c r="E46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" t="s">
+        <v>576</v>
+      </c>
+      <c r="C47" t="s">
+        <v>981</v>
+      </c>
+      <c r="D47" t="s">
+        <v>982</v>
+      </c>
+      <c r="E47" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>981</v>
+      </c>
+      <c r="D48" t="s">
+        <v>982</v>
+      </c>
+      <c r="E48" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>981</v>
+      </c>
+      <c r="D49" t="s">
+        <v>982</v>
+      </c>
+      <c r="E49" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>981</v>
+      </c>
+      <c r="D50" t="s">
+        <v>982</v>
+      </c>
+      <c r="E50" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" t="s">
+        <v>981</v>
+      </c>
+      <c r="D51" t="s">
+        <v>982</v>
+      </c>
+      <c r="E51" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
+        <v>396</v>
+      </c>
+      <c r="C52" t="s">
+        <v>981</v>
+      </c>
+      <c r="D52" t="s">
+        <v>982</v>
+      </c>
+      <c r="E52" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>981</v>
+      </c>
+      <c r="D53" t="s">
+        <v>982</v>
+      </c>
+      <c r="E53" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>550</v>
+      </c>
+      <c r="C54" t="s">
+        <v>981</v>
+      </c>
+      <c r="D54" t="s">
+        <v>982</v>
+      </c>
+      <c r="E54" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>981</v>
+      </c>
+      <c r="D55" t="s">
+        <v>982</v>
+      </c>
+      <c r="E55" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D419"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="B304" sqref="B304"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -27063,7 +28926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C440"/>
   <sheetViews>
@@ -31927,7 +33790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B96"/>
   <sheetViews>
@@ -32720,11 +34583,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>

</xml_diff>